<commit_message>
transform all cells in the dataframe in str
</commit_message>
<xml_diff>
--- a/NewSongs.xlsx
+++ b/NewSongs.xlsx
@@ -1191,19 +1191,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1247,17 +1241,17 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="20" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="20" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1577,7 +1571,7 @@
     <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1595,7 +1589,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1613,7 +1607,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1631,7 +1625,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -1649,7 +1643,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1667,7 +1661,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1685,7 +1679,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1703,7 +1697,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1721,7 +1715,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -1739,7 +1733,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
@@ -1757,7 +1751,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -1775,7 +1769,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -1793,7 +1787,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -1811,7 +1805,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
@@ -1829,7 +1823,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
On enlève les espaces et les chiffres
</commit_message>
<xml_diff>
--- a/NewSongs.xlsx
+++ b/NewSongs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b996519c3fe9888/Documents/GitHub/songRecommandation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_D0D0EC51E48CC2E6CF6DA46AEEBC070891CB7EEF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6850A8A-DB47-4075-A719-D761368D3F04}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="11_D0D0EC51E48CC2E6CF6DA46AEEBC070891CB7EEF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCF0D855-5045-4CFB-B882-45BA54D36B54}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="390">
   <si>
     <t>title</t>
   </si>
@@ -103,18 +103,12 @@
     <t>Memories</t>
   </si>
   <si>
-    <t xml:space="preserve">Maroon 5 </t>
-  </si>
-  <si>
     <t>JORDI</t>
   </si>
   <si>
     <t>Here's to the ones that we got||Cheers to the wish you were here, but you're not||'Cause the drinks bring back all the memories||Of everything we've been through||Toast to the ones here today||Toast to the ones that we lost on the way||'Cause the drinks bring back all the memories||And the memories bring back, memories bring back you||There's a time that I remember when I did not know no pain||When I believed in forever and everything would stay the same||Now my heart feel like December when somebody say your name||'Cause I can't reach out to call you, but I know I will one day, yeah||Everybody hurts sometimes||Everybody hurts someday, ayy-ayy||But everything gon' be alright||Go and raise a glass and say, ayy||Here's to the ones that we got||Cheers to the wish you were here, but you're not||'Cause the drinks bring back all the memories||Of everything we've been through||Toast to the ones here today||Toast to the ones that we lost on the way||'Cause the drinks bring back all the memories||And the memories bring back, memories bring back you||Doo-doo, doo-doo-doo-doo||Doo-doo-doo-doo, doo-doo-doo-doo||Doo-doo-doo-doo, doo-doo-doo||Memories bring back, memories bring back you||There's a time that I remember when I never felt so lost||When I felt all of the hatred was too powerful to stop (Ooh, yeah)||Now my heart feel like an ember and it's lighting up the dark||I'll carry these torches for ya that you know I'll never drop, yeah||Everybody hurts sometimes||Everybody hurts someday, ayy-ayy||But everything gon' be alright||Go and raise a glass and say, ayy||Here's to the ones that we got (Oh-oh)||Cheers to the wish you were here, but you're not||'Cause the drinks bring back all the memories||Of everything we've been through (No, no)||Toast to the ones here today (Ayy)||Toast to the ones that we lost on the way||'Cause the drinks bring back all the memories (Ayy)||And the memories bring back, memories bring back you||Doo-doo, doo-doo-doo-doo||Doo-doo-doo-doo, doo-doo-doo-doo||Doo-doo-doo-doo, doo-doo-doo||Memories bring back, memories bring back you||Doo-doo, doo-doo-doo-doo||Doo-doo-doo-doo, doo-doo-doo-doo||Doo-doo-doo-doo, doo-doo-doo (Ooh, yeah)||Memories bring back, memories bring back you||Yeah, yeah, yeah||Yeah, yeah, yeah, yeah, yeah, no, no||Memories bring back, memories bring back you</t>
   </si>
   <si>
-    <t xml:space="preserve"> Follow You</t>
-  </si>
-  <si>
     <t xml:space="preserve">Imagine Dragons </t>
   </si>
   <si>
@@ -124,9 +118,6 @@
     <t>You know I got your number, number all night||I'm always on your team, I got your back, alright||Taking those, taking those losses if he treats you right||I wanna put you into the spotlight||If the world would only know what you've been holding back||Heart attacks every night||Oh, you know it's not right||I will follow you way down wherever you may go||I'll follow you way down to your deepest low||I'll always be around wherever life takes you||You know I'll follow you||Call you up, you've been crying, crying all night||You're only disappointed in yourself, alright||Taking those, taking those losses if it treats you right||I wanna take you into the sunlight||If the world would only know what you've been holding back||Heart attacks every night||Oh, you know it's not right||I will follow you way down wherever you may go||I'll follow you way down to your deepеst low||I'll always be around wherevеr life takes you||You know I'll follow you||La-da-da-da-da-da, la-da-da-da-da-da||La-da-da-da-da-da, you know I'll follow you||La-da-da-da-da-da, wherever life takes you||You know I'll follow you||You're not the type to give yourself enough love||She live her life, hand in a tight glove||I wish that I could fix it, I could fix it for you||But instead I'll be right here comin' through||(Right here coming through)||I will follow you way down wherever you may go (I'll follow you)||I'll follow you way down to your deepest low||I'll always be around wherever life takes you (I'll follow you)||You know I'll follow you||La-da-da-da-da-da, la-da-da-da-da-da||La-da-da-da-da-da, you know I'll follow you||La-da-da-da-da-da, wherever life takes you||You know I'll follow you</t>
   </si>
   <si>
-    <t xml:space="preserve"> Best Song Ever</t>
-  </si>
-  <si>
     <t xml:space="preserve">One Direction </t>
   </si>
   <si>
@@ -145,18 +136,12 @@
     <t>When I find myself in times of trouble||Mother Mary comes to me||Speaking words of wisdom||Let it be||And in my hour of darkness||She is standing right in front of me||Speaking words of wisdom||Let it be||Let it be, let it be||Let it be, let it be||Whisper words of wisdom||Let it be||And when the broken hearted||People living in the world agree||There will be an answer||Let it be||For though they may be parted||There is still a chance that they will see||There will be an answer||Let it be||Let it be, let it be||Let it be, let it be||Yeah, there will be an answer||Let it be||Let it be, let it be||Let it be, let it be||Whisper words of wisdom||Let it be||Let it be, let it be||Let it be, yeah, let it be||Whisper words of wisdom||Let it be||And when the night is cloudy||There is still a light that shines on me||Shine until tomorrow||Let it be||I wake up to the sound of music||Mother Mary comes to me||Speaking words of wisdom||Let it be, yeah||Let it be, let it be||Let it be, yeah, let it be||Oh, there will be an answer||Let it be||Let it be, let it be||Let it be, yeah, let it be||Oh, there will be an answer||Let it be||Let it be, let it be||Let it be, yeah, let it be||Whisper words of wisdom||Let it be</t>
   </si>
   <si>
-    <t xml:space="preserve"> Beggin'</t>
-  </si>
-  <si>
     <t>Beggin'</t>
   </si>
   <si>
     <t>Put your lovin' hand out, baby||'Cause I'm beggin'||I'm beggin', beggin' you||So put your loving hand out, baby||I'm beggin', beggin' you||So put your loving hand out, darlin'||Riding high when I was king||I played it hard and fast, 'cause I had everything||I walked away, you won me then||But easy come and easy go and it would end||So anytime I bleed, you let me go||Yah, anytime I feed, you get me, no||Anytime I seek, you let me know||But I plant and seed, just let me go||I'm on my knees when I'm beggin'||'Cause I don't wanna lose you||Hey, yeah, ra-ta-ta-ta!||'Cause I'm beggin', beggin' you||Uh, put your loving hand out, baby||I'm beggin', beggin' you, ah||And put your loving hand out, darlin'||I need you to understand||Tried so hard to be your man||The kind of man you want in the end||Only then can I begin to live again||An empty shell, I used to be||The shadow of my life was hangin' over me||A broken man that I don't know||Won't even stand the devil's dance to win my soul||What we doin'? What we chasin'?||Why the bottom? Why the basement?||Why we got good shit, don't embrace it?||Why the feel for the need to replace me?||You're the wrong way track from the good||I want to paint a picture tellin' where we could be at||Like a heart in the best way should||You can give it away, you had it and you took the pay||But I keep walkin' on, keep openin' doors||Keep hopin' for, now the door is yours||Keep also home||'Cause I don't wanna live in a broken home, girl, I'm beggin'||Mmm, yeah, yeah, I'm beggin', beggin' you||So put your loving hand out, baby||I'm beggin', beggin' you||So put your loving hand out, darlin'||I'm fighting hard to hold my own||Just can't make it all alone||I'm holdin' on, I can't fall back||I'm just a calm, 'bout to fade to black||I'm beggin', beggin' you||Put your loving hand out, baby||I'm beggin', beggin' you||So put your loving hand out, darlin'||I'm beggin', beggin' you||So put your loving hand out, baby||I'm beggin', beggin' you||So put your loving hand out, darlin'||I'm beggin', beggin' you||So put your loving hand out, baby||I'm beggin', beggin' you||So put your loving hand out</t>
   </si>
   <si>
-    <t xml:space="preserve"> Why'd You Only Call Me When You're High?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Arctic Monkeys </t>
   </si>
   <si>
@@ -166,9 +151,6 @@
     <t>The mirror's image tells me it's home time||But I'm not finished, 'cause you're not by my side||And as I arrived I thought I saw you leavin'||Carryin' your shoes||Decided that once again I was just dreamin'||Of bumpin' into you||Now, it's three in the mornin'||And I'm tryna' change your mind||Left you multiple missed calls||And to my message, you reply||"Why'd you only call me when you're high?"||"Hi, why'd you only call me when you're high?"||Somewhere darker, talkin' the same shite||I need a partner, (High) well are you out tonight?||It's harder and harder to get you to listen||More I get through the gears||Incapable of makin' alright decisions||And having bad ideas||Now, it's three in the mornin'||And I'm tryna' change your mind||Left you multiple missed calls||And to my message, you reply (Message, you reply)||"Why'd you only call me when you're high?"||(Why'd you only call me when you're)||"Hi, why'd you only call me when you're high?"||And I can't see you here, wonder where I might||It sort of feels like I'm runnin' out of time||I haven't found all I was hopin' to find||You said you got to be up in the mornin'||Gonna have an early night||And you're startin' to bore me, baby||"Why'd you only call me when you're high?"||"Why'd you only ever phone me when you're high?"||"Why'd you only ever phone me when you're high?"||"Why'd you only ever phone me when you're high?"||"Why'd you only ever phone me when you're (high)?"</t>
   </si>
   <si>
-    <t xml:space="preserve"> In the End</t>
-  </si>
-  <si>
     <t xml:space="preserve">Linkin Park </t>
   </si>
   <si>
@@ -184,9 +166,6 @@
     <t>Come a little closer 'cause you lookin' thirsty||I'ma make it better, sip it like a Slurpee||Snow cone chilly, get it free like Willy (Oh)||In the jeans like Billie, you be poppin' like a wheelie||Even in the sun, you know I keep it icy||You could take a lick, but it's too cold to bite me (Haha)||Brr, brr, frozen, you're the one been chosen||Play the part like Moses, keep it fresh like roses (Oh)||Look so good, yeah, look so sweet (Hey)||Lookin' good enough to eat||Coldest with the kiss, so he call me ice cream||Catch me in the fridge, right where the ice be||Look so good, yeah, look so sweet (Hey)||Baby, you deserve a treat||Diamonds on my wrist, so he call me ice cream||You could double-dip 'cause I know you like me||Ice cream chillin', chillin', ice cream chillin'||Ice cream chillin', chillin', ice cream chillin'||I know that my heart can be so cold||But I'm sweet for you, come put me in a cone (In a cone)||You're the only touch, yeah, that get me meltin'||He's my favorite flavor, always gonna pick him||You're the cherry piece, just stay on top of me, so||I can't see nobody else for me, no||Get it, flip it, scoop it, do it like that, oh yeah, oh yeah||Like it, love it, lick it, do it like la-la-la, oh yeah||Look so good, yeah, look so sweet (Hey)||Lookin' good enough to eat||Coldest with the kiss, so he call me ice cream||Catch me in the fridge, right where the ice be||Look so good, yeah, look so sweet (Hey)||Baby, you deserve a treat||Diamonds on my wrist, so he call me ice cream||You could double-dip 'cause I know you like me||Ice cream chillin', chillin', ice cream chillin'||Ice cream chillin', chillin', ice cream chillin'||Ice cream chillin', chillin', ice cream chillin'||Ice cream chillin', chillin', ice cream||Chillin' like a villain, yeah, ra-ra-ra||미친 미친듯한 속도 in my La Ferra'||너무 빨러 너는 삐끗 원한다면 그냥 지름||Millis, billis 매일 벌음 한여름 손목에 얼음||Keep it movin' like my lease up||Think you fly, boy, where your visa?||Mona Lisa kinda Lisa||Needs an ice cream man that treats her||Keep it movin' like my lease up||Think you fly, boy, where your visa?||Mona Lisa kinda Lisa||Needs an ice cream man that treats her (Hey)||Na, na-na-na-na||Na, na-na-na-na (Hey)||Ice on my wrist, yeah, I like it like this||Get the bag with the cream||If you know what I mean||Ice cream, ice cream, ice cream chillin'||Na, na-na-na-na||Na, na-na-na-na (Hey)||Ice on my wrist, yeah, I like it like this||And I'm nice with the cream||If you know what I mean||Ice cream, ice cream||Ice cream</t>
   </si>
   <si>
-    <t xml:space="preserve"> Shy Away</t>
-  </si>
-  <si>
     <t xml:space="preserve">Twenty One Pilots </t>
   </si>
   <si>
@@ -196,9 +175,6 @@
     <t>When I get home||You better not be there||We're placin' bets you won't||Shed your modesty||And the only thing to leave behind||Is your own skin on the floor||Don't you shy away (Ah-ah-ah)||Manifest a ceiling||When you shy away (Ah-ah-ah)||Searchin' for that feelin'||Just like an "I love you" (Ooh, ooh)||That isn't words (Ooh, ooh)||Like a song he wrote that's never heard (Ah-ah-ah)||Don't you sh…||When you get home||You barely recognize the pictures||They put in a frame||'Cause you shed your modеsty||Don't circle the track||Take what you havе||And leave your skin on the floor||Don't you shy away (Ah-ah-ah)||Manifest a ceiling||When you shy away (Ah-ah-ah)||Searchin' for that feelin'||Just like an "I love you" (Ooh, ooh)||That isn't words (Ooh, ooh)||Like a song he wrote (Ah-ah-ah)||That's never heard||When I get home||Boy, you better not be there||You're long gone||Shed your modesty||Don't circle the track||Just break the cycle in half||And leave your skin on the floor||Don't you shy away (Ah-ah-ah)||Manifest a ceiling||When you shy away (Ah-ah-ah)||Searchin' for that feelin'||Just like an "I love you" (Ooh, ooh)||That isn't words (Ooh, ooh)||Like a song he wrote (Ah-ah-ah)||That's never heard||That's never heard (Ah-ah-ah, ah-ah-ah)||An "I love you"||That isn't words||Like a song he wrote||That's never heard||Don't you shy away</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sweater Weather</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Neighbourhood </t>
   </si>
   <si>
@@ -208,9 +184,6 @@
     <t>And all I am is a man||I want the world in my hands||I hate the beach, but I stand||In California with my toes in the sand||Use the sleeves of my sweater, let's have an adventure||Head in the clouds, but my gravity's centered||Touch my neck and I'll touch yours||You in those little high-waisted shorts, oh||She knows what I think about||And what I think about||One love, two mouths||One love, one house||No shirt, no blouse||Just us, you find out||Nothing that I wouldn't wanna tell you about, no||'Cause it's too cold for you here and now||So let me hold both your hands in the holes of my sweater||And if I may just take your breath away||I don't mind if there's not much to say||Sometimes the silence guides a mind||To move to a place so far away||The goosebumps start to raise||The minute that my left hand meets your waist||And then I watch your face||Put my finger on your tongue 'cause you love the taste, yeah||These hearts adore||Everyone the other beats hardest for||Inside, this place is warm||Outside, it starts to pour||Comin' down||One love, two mouths||One love, one house||No shirt, no blouse||Just us, you find out||Nothin' that I wouldn't wanna tell you about||No, no, no||'Cause it's too cold for you here and now||So let me hold both your hands in the holes of my sweater||'Cause it's too cold for you here and now||So let me hold both your hands in the holes of my sweater||Woah||Woah, woah, woah||Woah, woah, woah, woah||Woah, woah||Woah, woah, woah, woah||Woah, woah||'Cause it's too cold for you here and now||So let me hold both your hands in the holes of my sweater||'Cause it's too cold for you here and now||Let me hold both your hands in the holes of my sweater||And it's too cold, it's too cold||The holes of my sweater</t>
   </si>
   <si>
-    <t xml:space="preserve"> Scar Tissue</t>
-  </si>
-  <si>
     <t xml:space="preserve">Red Hot Chili Peppers </t>
   </si>
   <si>
@@ -220,21 +193,12 @@
     <t>Scar tissue that I wish you saw||Sarcastic mister know-it-all||Close your eyes and I'll kiss you||'Cause with the birds I'll share||With the birds, I'll share this lonely view||With the birds, I'll share this lonely view||Ah, push me up against the wall||Young Kentucky girl in a push-up bra||Ah, fallin' all over myself||To lick your heart and taste your health, 'cause||With the birds (Share this lone—), I'll share this lonely view||With the birds (Share this lone—), I'll share this lonely view||With the birds (Share this lone—), I'll share this lonely view||Blood loss in a bathroom stall||A southern girl with a scarlet drawl||I wave good-bye to Ma and Pa||'Cause with the birds I'll share||With the birds (Share this lonely), I'll share this lonely view||With the birds (Share this lonely), I'll share this lonely view||Soft-spoken with a broken jaw||Step outside but not to brawl and||Autumn's sweet, we call it fall||I'll make it to the moon if I have to crawl and||(I will share this lonely)||With the birds, I'll share this lonely view||(I will share this lonely)||With the birds, I'll share this lonely view||(I will share this lonely)||With the birds, I'll share this lonely view||Scar tissue that I wish you saw||Sarcastic mister know-it-all||Close your eyes and I'll kiss you||'Cause with the birds I'll share||(I will share this lonely)||With the birds, I'll share this lonely view||(I will share this lonely)||With the birds, I'll share this lonely view||(I will share this lonely)||With the birds, I'll share this lonely view</t>
   </si>
   <si>
-    <t xml:space="preserve"> Thunderstruck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC/DC </t>
-  </si>
-  <si>
     <t>The Razors Edge</t>
   </si>
   <si>
     <t>Thunder, ah||Thunder, ah||Thunder, ah||Thunder, ah||Thunder, ah||Thunder, ah||Thunder, ah||Thunder, ah||Thunder, ah||Thunder, ah||I was caught||In the middle of a railroad track (Thunder)||I looked 'round||And I knew there was no turning back (Thunder)||My mind raced||And I thought, what could I do? (Thunder)||And I knew||There was no help, no help from you (Thunder)||Sound of the drums||Beating in my heart||The thunder of guns||Tore me apart||You've been - thunderstruck||Went down the highway||Broke the limit, we hit the town||Went through to Texas||Yeah, Texas, and we had some fun||We met some girls||Some dancers who gave a good time||Broke all the rules, played all the fools||Yeah-yeah, they, they, they blew our minds||I was shaking at the knees||Could I come again please?||Yeah, the ladies were too kind||You've been - thunderstruck, thunderstruck||Yeah-yeah-yeah, thunderstruck||Oh, thunderstruck||Yeah||I was shaking at the knees||Could I come again please?||Yow||Thunderstruck, thunderstruck||Yeah-yeah-yeah, thunderstruck||Thunderstruck, yeah, yeah, yeah||Said||Yeah, it's alright||We're doing fine||Yeah, it's alright||We're doing fine, so fine||Thunderstruck, yeah-yeah-yeah||Thunderstruck, thunderstruck, thunderstruck||Whoa, baby, baby (Thunderstruck)||You've been thunderstruck, thunderstruck||Thunderstruck, thunderstruck||You've been thunderstruck</t>
   </si>
   <si>
-    <t xml:space="preserve"> I Gotta Feeling</t>
-  </si>
-  <si>
     <t xml:space="preserve">Black Eyed Peas </t>
   </si>
   <si>
@@ -244,9 +208,6 @@
     <t>I got a feeling||That tonight's gonna be a good night||That tonight's gonna be a good night||That tonight's gonna be a good, good night||A feeling||That tonight's gonna be a good night||That tonight's gonna be a good night||That tonight's gonna be a good, good night||A feeling, woo-hoo||That tonight's gonna be a good night||That tonight's gonna be a good night||That tonight's gonna be a good, good nightA feeling, woo-hoo||That tonight's gonna be a good night||That tonight's gonna be a good night||That tonight's gonna be a good, good night (A feel-)||Tonight's the night||Let's live it up||I got my money||Let's spend it up (I feel-)||Go out and smash it||Like oh my God||Jump off that sofa||Let's kick it off (I feel-)||I know that we'll have a ball||If we get down and go out and just lose it all||I feel stressed out, I wanna let it go||Let's go way out, spaced out||And losin' all control (I feel-)||Fill up my cup||Mazel tov||Look at her dancin'||Just take it off (I feel-)||Let's paint the town||We'll shut it down||Let's burn the roof||And then we'll do it again (I feel-)||Let's do it, let's do it, let's do it, let's do it||And do it, and do it, let's live it up||And do it, and do it, and do it, do it, do it||Let's do it, let's do it, let's do it||'Cause I got a feeling, woo-hoo||That tonight's gonna be a good night||That tonight's gonna be a good night||That tonight's gonna be a good, good night||A feeling, woo-hoo||That tonight's gonna be a good night||That tonight's gonna be a good night||That tonight's gonna be a good, good night (A feel-)||Tonight's the night (Hey)||Let's live it up (Let's live it up)||I got my money (I'm paying)||Let's spend it up (Let's spend it up)||Go out and smash it (Smash it)||Like oh my God (Like oh my God)||Jump off that sofa (Come on)||Let's kick it off||Fill up my cup (Drank)||Mazel tov (L'chaim)||Look at her dancin' (Move it, move it)||Just take it off||Let's paint the town (Paint the town)||We'll shut it down (Shut it down)||Let's burn the roof||And then we'll do it again||Let's do it, let's do it, let's do it, let's do it (Let's do it)||And do it (do it), and do it, let's live it up||And do it (do it), and do it (and do it)||And do it (and), do it (and), do it (and do it)||Let's do it (and do it), let's do it (and do it)||Let's do it (hey), do it (hey), do it (hey), do it||Here we come, here we go||We gotta rock||Easy come, easy go||Now we on top||Fill the shot, body rock||Rock it, don't stop||Round and round, up and down||Around the clock||Monday, Tuesday, Wednesday and Thursday (Do it)||Friday, Saturday, Saturday to Sunday (Do it)||Get, get, get, get with us||You know what we say||Party every day||P-p-p-party every day||And I'm feeling, woo-hoo||That tonight's gonna be a good night||That tonight's gonna be a good night||That tonight's gonna be a good, good night||A feeling, woo-hoo||That tonight's gonna be a good night||That tonight's gonna be a good night||That tonight's gonna be a good, good night||Woo-hoo</t>
   </si>
   <si>
-    <t xml:space="preserve"> Someday</t>
-  </si>
-  <si>
     <t xml:space="preserve">OneRepublic </t>
   </si>
   <si>
@@ -256,9 +217,6 @@
     <t>Some days, I'm treadin' the water||And feel like it's gettin' deep||Some nights, I drown in the weight||Of the things that I think I need||Sometimes, I feel incomplete, yeah||But you always say to me, say to me||Oh, you say someday, when we're older||We'll be shinin' like we're gold||Yeah, won't we? (Won't we?) Won't we? (Won't we?)||Yeah, someday, when we're older||I'll be yours and you'll be mine||Babe, happy (Happy), happy||Oh, you say someday, when we're older||We won't worry 'bout the things||That we don't need (We don't need), we don't need (Oh)||Yeah, one day, down the line||Before we both run out of time, you're gonna see||That someday, we'll be all that we need||Someday, we'll be all that we need||I've been the best, been the worst||Been a ghost in a crowded room (Oh, yeah-yeah-yeah-yeah-yeah)||I took a chance, took a turn||Took a dive, and it led to you (Oh, yeah-yeah-yeah-yeah-yeah)||So many times that I wish||We could be anywhere but here||So many times that I wish||I could see what you see so clear, so clear||Oh, you say someday, when we're older||We'll be shinin' like we're gold||Yeah, won't we? (Won't we?) Won't we? (Won't we?) Yeah||Yeah, someday, when we're older||I'll be yours and you'll be mine||Babe, happy (Happy), happy||Oh, you say someday, when we're older||We won't worry 'bout the things||That we don't need (We don't need), we don't need (Oh)||Yeah, one day, down the line||Before we both run out of time, you're gonna see||That someday, we'll be all that we need||Someday, we'll be all that we need||Oh, you say someday, when we're older||We'll be shinin' like we're gold||Yeah, won't we? Won't we?||Mm, someday, down the line||Before we both run out of time, you're gonna see||That someday, we'll be all that we need</t>
   </si>
   <si>
-    <t xml:space="preserve"> Enter Sandman</t>
-  </si>
-  <si>
     <t xml:space="preserve">Metallica </t>
   </si>
   <si>
@@ -268,9 +226,6 @@
     <t>Say your prayers, little one, don't forget, my son||To include everyone||I tuck you in, warm within, keep you free from sin||'Til the Sandman, he comes||Sleep with one eye open||Gripping your pillow tight||Exit light||Enter night||Take my hand||We're off to never-never land||Something's wrong, shut the light, heavy thoughts tonight||And they aren't of Snow White||Dreams of war, dreams of liars, dreams of dragons' fire||And of things that will bite, yeah||Sleep with one eye open||Gripping your pillow tight||Exit light||Enter night||Take my hand||We're off to never-never land||Yeah-hah||Now, I lay me down to sleep (Now, I lay me down to sleep)||Pray the Lord my soul to keep (Pray the Lord my soul to keep)||If I die before I wake (If I die before I wake)||Pray the Lord my soul to take (Pray the Lord my soul to take)||Hush, little baby, don't say a word||And never mind that noise you heard||It's just the beasts under your bed||In your closet, in your head||Exit light||Enter night||Grain of sand||Exit light||Enter night||Take my hand||We're off to never-never land (yeah, haha haha)||Oh! Yeah-yeah, yo-oh||We're off to never-never land||Take my hand||We're off to never-never land||Take my hand||We're off to never-never land||We're off to never-never land||We're off to never-never land||We're off to never-never land</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sweet Melody</t>
-  </si>
-  <si>
     <t xml:space="preserve">Little Mix </t>
   </si>
   <si>
@@ -280,18 +235,12 @@
     <t>Doo-doo, doo-doo-doo-doo||Doo-roo-doo-doo, doo-roo-doo-roo||Doo-doo, doo-doo-doo-doo||Doo-roo-doo-doo, doo-doo-doo-doo||In a whole 'nother life, there was this boy that I knew||He made me feel like a woman, we were young and silly fools||Anyway, he was in a band, wrote love songs about me||I wasn't crazy 'bout the words, but the melodies were sweet||Went something like||Doo-doo, doo-doo-doo-doo||Doo-roo-doo-doo, doo-roo-doo-roo||Doo-doo, doo-doo-doo-doo||Doo-roo-doo-doo, doo-doo-doo-doo||Every time we'd go dancing, I'd see his straying eyes||Gave him too many chances, pushed my keys too many times||Anyway, he'd start actin' up, and I'd be on my way to leave (Ooh)||But I stopped in my tracks when I heard this melody||And it went like||Doo-doo, doo-doo-doo-doo||Doo-roo-doo-doo, doo-roo-doo-roo||Doo-doo, doo-doo-doo-doo||Doo-roo-doo-doo, doo-doo-doo-doo||He used to sing me sweet melodies||He played me, made me believe it was real love||Sang me sweet melodies||But the day he did me wrong||The song couldn't go on and on and on||He used to sing me sweet melodies||He played me, made me believe it was real love||Sang me sweet melodies||But the day he did me wrong||The song couldn't go on and on and on||He would lie, he would cheat, over syncopated beats||I was just his tiny dancer, he had control of my feet||Yes, when he came along, that's when I lost a groove||There was no song in the world to sing along or make me move||Sounded something like||Doo-doo, doo-doo-doo-doo (Ooh)||Doo-roo-doo-doo, doo-roo-doo-roo (It was)||Doo-doo, doo-doo-doo-doo (Ooh)||Doo-roo-doo-doo, doo-doo-doo-doo (Oh)||He used to sing me sweet melodies (Oh, woah)||He played me, made me believe it was real love||Sang me sweet melodies||But the day he did me wrong (Ah, yeah)||The song couldn't go on and on and on (Couldn't go on, no)||He used to sing me sweet melodies (Sweet, sweet melodies)||He played me, made me believe it was real love (Real love)||Sang me sweet melodies||But the day he did me wrong (Me wrong)||The song couldn't go on and on and on (On and on and on)||Doo-doo, doo-doo-doo-doo (Ooh; Ayy, ayy)||Doo-roo-doo-doo, doo-roo-doo-roo (Oh)||Doo-doo, doo-doo-doo-doo (Ooh)||Doo-roo-doo-doo, doo-roo-doo-roo (Oh, woah)||On and on (Oh-oh-oh)||On and on (Oh-oh-oh)||He used to sing me sweet melodies (Oh-oh-oh)||He played me, made me believe it was real love (Oh-oh-oh)||Sang me sweet melodies (Oh-oh-oh)||But the day he did me wrong (Me wrong)||The song couldn't go on and on and on||On and on and on, yeah||He used to sing me sweet melodies (Melodies, yeah)||He played me, made me believe it was real love (Real love)||Sang me sweet melodies (Oh-oh)||But the day he did me wrong (Did me wrong)||The song couldn't go on and on and on (On and on, yeah)||He used to sing me sweet melodies (Sing me sweet melodies, yeah)||He played me (Made me believe), made me believe it was real love (It was real love, oh)||Sang me sweet melodies (*Oh*)||But the day he did me wrong (Eh)||The song couldn't go *on and on and on, no*</t>
   </si>
   <si>
-    <t xml:space="preserve"> Takeaway</t>
-  </si>
-  <si>
     <t>World War Joy</t>
   </si>
   <si>
     <t>Your heart for takeaway, yeah, yeah, yeah-yeah||Your heart for takeaway, yeah, yeah, yeah-yeah||Your heart for takeaway, yeah-yeah, yeah-yeah||Your heart for takeaway, yeah, yeah, yeah-yeah||Hey, hey, hey||Where do you think you're going||It's so late, late, late, what's wrong?||I said, "I can't stay, do I have to give a reason?"||It's just me, me, me, it's what I want||So how did we get here?||Three weeks now, we've been so caught up||Better if we do this on our own||Before I love you, na-na-na||I'm gonna leave you, na-na-na||Before I'm someone you leave behind||I'll break your heart so you don't break mine||Before I love you, na-na-na||I'm gonna leave you, na-na-na||Even if I'm not here to stay||I still want your heart||Your heart for takeaway, yeah, yeah, yeah-yeah||Your heart for takeaway, yeah, yeah, yeah-yeah||Your heart for takeaway, yeah-yeah, yeah-yeah||Your heart for takeaway, yeah, yeah, yeah-yeah||Your heart for takeaway||(Your heart for takeaway, yeah-yeah, yeah-yeah)||Your heart for takeaway, yeah, yeah, yeah-yeah||Fate, fate, fate||Is that what came between us?||Or did we do this on our own?||So how did we get here?||I'm asking myself why I'm so caught up||Better if we do this on our own||Before I love you, na-na-na||I'm gonna leave you, na-na-na||Before I'm someone you leave behind||I'll break your heart so you don't break mine||Before I love you, na-na-na||I'm gonna leave you, na-na-na||Even if I'm not here to stay||I still want your heart</t>
   </si>
   <si>
-    <t xml:space="preserve"> Heat Waves</t>
-  </si>
-  <si>
     <t xml:space="preserve">Glass Animals </t>
   </si>
   <si>
@@ -301,9 +250,6 @@
     <t>(Last night, all I think about is you)||(Don't stop, baby, you can walk through)||(Don't want, baby, think about you)||(You know that I'm never gonna lose)||Road shimmer wigglin' the vision||Heat, heat waves, I'm swimmin' in a mirror||Road shimmer wigglin' the vision||Heat, heat waves, I'm swimmin' in a—||Sometimes, all I think about is you||Late nights in the middle of June||Heat waves been fakin' me out||Can't make you happier now||Sometimes, all I think about is you||Late nights in the middle of June||Heat waves been fakin' me out||Can't make you happier now||Usually, I put somethin' on TV||So we never think about you and me||But today, I see our reflections clearly||In Hollywood, layin' on the screen||You just need a better life than this||You need somethin' I can never give||Fake water all across the road||It's gone now, the night has come, but||Sometimes, all I think about is you||Late nights in the middle of June||Heat waves been fakin' me out||Can't make you happier now||You can't fight it, you can't breathe||You say somethin' so lovin', but||Now I gotta let you go||You'll be better off in someone new||I don't wanna be alone||You know it hurts me too||You look so broken when you cry||One more and then I say goodbye||Sometimes, all I think about is you||Late nights in the middle of June||Heat waves been fakin' me out||Can't make you happier now||Sometimes, all I think about is you||Late nights in the middle of June||Heat waves been fakin' me out||Can't make you happier now||I just wonder what you're dreamin' of||When you sleep and smile so comfortable||I just wish that I could give you that||That look that's perfectly un-sad||Sometimes, all I think about is you||Late nights in the middle of June||Heat waves been fakin' me out||Heat waves been fakin' me out||Sometimes, all I think about is you||Late nights in the middle of June||Heat waves been fakin' me out||Can't make you happier now||Sometimes, all I think about is you||Late nights in the middle of June||Heat waves been fakin' me out||Can't make you happier now||Road shimmer wigglin' the vision||Heat, heat waves, I'm swimmin' in a mirror||Road shimmer wigglin' the vision||Heat, heat waves, I'm swimmin' in a mirror</t>
   </si>
   <si>
-    <t xml:space="preserve"> The Feels</t>
-  </si>
-  <si>
     <t xml:space="preserve">TWICE </t>
   </si>
   <si>
@@ -313,9 +259,6 @@
     <t>Boy, I, boy, I, boy, I know||I know you get the feels (Yeah)||Boy, I, boy, I, boy, I know||Uh, I'm so curious||’Bout ya boy, wanna keep it cool||But I know everytime you move||Got me frozen, I||Get so shy, it's obvious (Yeah, yeah)||Catching feels like butterflies||If I say what's on my mind||Would I hit bullseye? (Woo)||Shoot! I’m ready, aim and fire (Fire!)||Baby, I (Woah, wow)||Feel like Cupid's alive||Ali-i-ive tonight||Yeah, tonight||If your heart beats the same way||Let me know (Yeah, let me know)||'Cause I'm boom-boom-boom||From head to toe and I (From head to toe)||I know love||It is such a funny thing||A mystery allure||Gotta get to know you more||'Cause I, I can feel a real connection||A supernatural attraction-ah||I got the feels for you, yeah, yeah, yeah, yeah||You have stolen my heart, oh, yeah (Oh, yeah)||Never let it go-oh-oh||No, never let it go-oh, oh-oh, oh-oh, oh||Lightning straight to my heart, oh, yeah (Oh, yeah)||I got all the feels for sure||Yeah, I got all the feels for ya||Boy, I, boy, I, boy, I know||I know I get the feels||Boy, I, boy, I, boy, I know||I know you feel it too||(Uh-uh)||Sway in the moonlight, dance in the dark (Yeah, yeah)||I, I know that I caught your eye (That's right)||Are we on the same vibe? (Same vibe)||I wonder what's on your mind||'Cause you got me good and I wanna be ya boo||If it’s dumb, well, I wanna be a fool (Woo, woo, woo!)||Underneath the neon lights, baby||Electricity tonight, baby||[Pre-Chorus: Mina, Chaeyoung, Jeongyeon, Jihyo]||I know love||It is such a funny thing (Yeah)||A mystery allure||Gotta get to know you more (No)||’Cause I, I can feel a real connection (Connection)||A supernatural attraction-ah (Attraction, ah)||I got the feels for you, yeah, yeah, yeah, yeah (Ah)||You have stolen my heart, oh, yeah (Oh, yeah)||Never let it go-oh-oh||No, never let it go-oh, oh-oh, oh-oh, oh||Lightning straight to my heart, oh, yeah (Oh, yeah)||I got all the feels for sure||Yeah, I got all the feels for ya (Oh, yeah)||Boy, I, boy, I, boy, I know||I know I get the feels||Boy, I, boy, I, boy, I know||I know you feel it too||Boy, I, boy, I, boy, I know||I know I get the feels||Boy, I, boy, I, boy, I know||I know you feel it too (Feel it too)||You got my attention (Oh)||So, what's your intention? (Oh)||Yeah, tell me, baby, what’s the deal?||Oh, one look and I know it||Baby, my eyes reveal||That you, you, you give me the feels, oh, yeah||You have stolen my heart, oh, yeah (Oh, yeah)||Never let it go-oh-oh (No, no)||No, never let it go-oh, oh-oh, oh-oh, oh (No, no)||Lightning straight to my heart, oh, yeah (Oh, yeah-ah, I)||I got all the feels for sure||Yeah, I got all the feels for ya||Boy, I, boy, I, boy, I know (The feels)||I know I get the feels (The feels) (Oh, yeah)||Boy, I, boy, I, boy, I know (Ayy) (Yeah, yeah, yeah)||I know you feel it too (Yeah, yeah, yeah)||Boy, I, boy, I, boy, I know (The feels) (The feels, come on)||I know I get the feels (The feels)||Boy, I, boy, I, boy, I know (Ayy)||I know you feel it too (Yeah)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Come As You Are</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nirvana </t>
   </si>
   <si>
@@ -325,9 +268,6 @@
     <t>Come as you are, as you were||As I want you to be||As a friend, as a friend||As an old enemy||Take your time, hurry up||Choice is yours, don't be late||Take a rest as a friend||As an old memoria||Memoria||Memoria||Memoria||Come doused in mud, soaked in bleach||As I want you to be||As a trend, as a friend||As an old memoria||Memoria||Memoria||Memoria||And I swear that I don't have a gun||No, I don't have a gun||No, I don't have a gun||'Ria||Memoria||Memoria||Memoria (No, I don't have a gun)||Well, I swear that I don't have a gun||No, I don't have a gun||No, I don't have a gun||No, I don't have a gun||No, I don't have a gun||(Memoria)||(Memoria)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Straightenin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Migos </t>
   </si>
   <si>
@@ -337,9 +277,6 @@
     <t>(DJ Durel)||(Ayy Castro, go crazy)||Yeah, (Soo) we gone (Huh), stop, we good (Stop)||Chill, we on, (Chyeah) scale, let's go (Let's go)||Domingo (Huh), let's go (Migo)||Take' (Huh), let’s go (Huh)||'Set (Huh), let’s roll||Straightenin', straightenin' (Woo)||Straightenin', yeah (Straight||Straightenin', straightenin' (Soo)||Straightenin', yeah (Straight)||Don't nothin' get straightenin' but straightenin' (Hey)||Don't nothin' get straightenin' but straightenin' (Soo)||Don't nothin' get straightenin' but straightenin' (Straight)||You don't get shit straight, you gon' straighten it (Nah)||In this game, sit back, be patient (Gang)||Niggas act like the gang went vacant (Huh?)||Niggas act like somеthing been taken (Took what?)||Ain't nothing but a little bit of straightenin' (I'm tеllin' ya)||Been kicking shit, poppin' out daily (Go)||On an island, it's a movie I'm making (That’s facts)||I'm counting dineros with Robert De Niro||He telling 'em that Cho amazing (Ayy)||Put that shit on (Shit on), niggas get shit on (Shit on)||I bought two whips, and I put my bitch on (Skrrt)||She put this wrist on (Wrist)||She factory set it with Richard Mille prongs (Ice)||Turn a pandemic into a bandemic||You know that’s the shit that we on (Yessir)||Them niggas gon' pull up and act like this shit is together||We don't fuck with you homes (Fuck 'em)||Uh uh, I don't do the fake kicking (No)||There go a rocket, is Take' in it? (Soo)||It's a problem with few then we straightenin' it (Straight)||Swap out the 'Cat, put a Demon in it (Skrrt)||Upgrade the bando, put fiends in it (Woo)||I got some shooters you ain't seen with me (Grrah)||We'll run that shit back, I just seen Tenet (Woah)||We're going to get straightenin'||Straightenin', straightenin' (Woo)||Straightenin', yeah (Straight)||Straightenin', straightenin' (Soo)||Straightenin', yeah (Straight)||Don't nothin' get straightenin' but straightenin' (Hey)||Don't nothin' get straightenin' but straightenin' (Soo)||Don't nothin' get straightenin' but straightenin' (Straight)||You don't get shit straight, you don't straighten it (Nah)||(Takeoff)||You don't get shit straight if you don't straighten it (No)||I'm the type to sit back and watch patient (Watch)||Do a trick with the stick, it's amazing (Stick)||In the bando trappin' out vacants (Bando)||Locs on like I'm starring in The Matrix (Matrix)||I keep the cookie like my grandma made it (Cookie)||I keep the keys and the pounds and the babies (Keys)||And the bricks came white like Shady (White)||Drive the Lambo' through the avenue (Skrrt)||Pretty lil bih' with a attitude (Bad)||Give a shoutout to the white boy (Boys)||All white Rolls look radical (Radical)||Keep you a fire, don't let 'em take it (No)||If they get yours you gotta get straightenin' (Straightenin')||I catch a opp, I give him a facelift (Opp)||My niggas lurkin' and spinnin' the day-shift (Lurk)||I got them racks when you see me (Rackaids)||Spin back to back, it's a repeat (Spin)||Championship, this a three-peat (Three)||Shoot out the window like Drizzy and Freaky (Freak)||I keep it on me, believe me (Yessir)||I be up high where the trees be (High)||I go and put on so much of this ice||They said "Don't touch me, you gon' freeze me" (Freeze)||Straightenin', straightenin' (Woo)||Straightenin', yeah (Straight)||Straightenin', straightenin' (Soo)||Straightenin', yeah (Straight)||Don't nothin' get straightenin' but straightenin' (Hey)||Don't nothin' get straightenin' but straightenin' (Soo)||Don't nothin' get straightenin' but straightenin' (Straight)||You don't get shit straight, you don't straighten it (Woo, woo, nah)||(Offset)||Get my straightenin' (Straightenin', get mine)||Automatic handgun like the Navy (Automatic, raow)||I keep a hundred-round drum, I ain't fading (Paow-paow-paow)||Turn a nigga to a mummy with the payment (Woo, woo)||Terminate him with the money (Hey!), it was gravy (Terminator)||Spin an opp block, rock-a-bye-baby (Rock-a-bye)||Made his heart stop, made his momma hate me (Make 'em hate me)||We were trappin' out the spot out the basement (Out the spot)||Tasmanian Devil, we spin on your block (Spin, ouch)||I pop a Perc' and I'm going berserk (Woah, woah)||And I woke up and bought me a drop (Like fuck it, eugh)||Straight to the point, I get straight to the straightenin' (Straight, straight)||Your buddy, he can't even walk (Straight, straight, straight)||We gutted up, nobody talk (We gutted up)||New Cullinan, stars start to fall (New Cullinan)||Trappin' and hustlin', beat down the walls (Beat down)||I'm with the steppa (Grr), Nawfside repper (Nawf)||Qua' keep a MAC in the back of the Tesla (MAC, Qua')||I'm with the gang (Gang), we could never be selfish (Gang-gang-gang)||Watch how I dress, I'm the drippin' professor||Sold the Kel-Tec, then I bought a compressor (Kel-Tec)||Time to press him, eat him for breakfast (Hey)||Taught him a lesson, I'm never confessing (Hey)||Left him a message, somebody stretch him (Stretch)||||Straightenin', straightenin' (Woo)||Straightenin', yeah (Straight)||Straightenin', straightenin' (Soo)||Straightenin', yeah (Straight)||Don't nothin' get straightenin' but straightenin' (Hey)||Don't nothin' get straightenin' but straightenin' (Soo)||Don't nothin' get straightenin' but straightenin' (Straight)||You don't get shit straight, you don't straighten it (Nah)||Straightenin'||No, nothin' get some straightenin' (Soo)||Yeah, don't nothin' get straightenin' but straightenin' (Don't nothin' get straightenin' but straightenin')||You feel me? (Don't nothin' get straight)||I don't know what y'all think goin' on out there but know what I mean? (Straightenin')||We straight, we straight (Don't nothin' get straight, yeah)||Soo, soo, soo, soo, soo, soo (Don't nothin' get straight)||We gone</t>
   </si>
   <si>
-    <t xml:space="preserve"> Boulevard of Broken Dreams</t>
-  </si>
-  <si>
     <t xml:space="preserve">Green Day </t>
   </si>
   <si>
@@ -349,24 +286,12 @@
     <t>I walk a lonely road||The only one that I have ever known||Don't know where it goes||But it's home to me, and I walk alone||I walk this empty street||On the Boulevard of Broken Dreams||Where the city sleeps||And I'm the only one, and I walk alone||I walk alone, I walk alone||I walk alone, I walk a—||My shadow's the only one that walks beside me||My shallow heart's the only thing that's beatin'||Sometimes, I wish someone out there will find me||'Til then, I walk alone||Ah-ah, ah-ah, ah-ah, ah-ah||Ah-ah, ah-ah, ah-ah||I'm walkin' down the line||That divides me somewhere in my mind||On the borderline||Of the edge and where I walk alone||Read between the lines||What's fucked up, and everything's all right||Check my vital signs||To know I'm still alive, and I walk alone||I walk alone, I walk alone||I walk alone, I walk a—||My shadow's the only one that walks beside me||My shallow heart's the only thing that's beatin'||Sometimes, I wish someone out there will find me||'Til then, I walk alone||Ah-ah, ah-ah, ah-ah, ah-ah||Ah-ah, ah-ah||I walk alone, I walk a—||I walk this empty street||On the Boulevard of Broken Dreams||Where the city sleeps||And I'm the only one, and I walk a—||My shadow's the only one that walks beside me||My shallow heart's the only thing that's beatin'||Sometimes, I wish someone out there will find me||'Til then, I walk alone</t>
   </si>
   <si>
-    <t xml:space="preserve"> Youngblood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 Seconds of Summer </t>
-  </si>
-  <si>
     <t>Youngblood</t>
   </si>
   <si>
     <t>Remember the words you told me||"Love me till the day I die"?||Surrender my everything||'Cause you made me believe you're mine||Yeah, you used to call me "baby"||Now, you're callin' me by name (Mm)||Takes one to know one, yeah||You beat me at my own damn game||You push and you push and I'm pullin' away||Pullin' away from ya||I give and I give and I give and you take||Give and you take||Youngblood||Say you want me, say you want me outta your life||And I'm just a dead man walkin' tonight||But you need it, yeah, you need it all of the time, yeah (Ooh)||Youngblood||Say you want me, say you want me back in your life||So I'm just a dead man crawlin' tonight||'Cause I need it, yeah, I need it all of the time, yeah (Ooh)||Lately, our conversations||End like it's the last goodbye||Then one of us gets too drunk||And calls about a hundred times||So who you been callin' "baby"?||Nobody could take my place||When you're lookin' at those strangers||Hope to God you see my face (Ooh)||Youngblood||Say you want me, say you want me outta your life||And I'm just a dead man walkin' tonight||But you need it, yeah, you need it all of the time, yeah (Ooh)||Youngblood||Say you want me, say you want me back in your life||So I'm just a dead man crawlin' tonight||'Cause I need it, yeah, I need it all of the time, yeah (Ooh)||You push and you push and I'm pullin' away||Pullin' away from ya||I give and I give and I give and you take||Give and you take||You're runnin' around and I'm runnin' away||Runnin' away from ya, mm, from ya||Youngblood||Say you want me, say you want me outta your life||And I'm just a dead man walkin' tonight||But you need it, yeah, you need it all of the time, yeah (Ooh)||Youngblood||Say you want me, say you want me back in your life||So I'm just a dead man crawlin' tonight||'Cause I need it, yeah, I need it all of the time, yeah (Ooh)||You push and you push and I'm pullin' away||Pullin' away from ya||I give and I give and I give and you take||Give and you take||Youngblood||Say you want me, say you want me outta your life||And I'm just a dead man walkin' tonight</t>
   </si>
   <si>
-    <t xml:space="preserve"> Chiquitita</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABBA </t>
-  </si>
-  <si>
     <t>Voulez-Vous</t>
   </si>
   <si>
@@ -382,9 +307,6 @@
     <t>If you start me up||If you start me up, I'll never stop||If you start me up||If you start me up, I'll never stop||I've been running hot||You got me ticking, now don't blow my top||If you start me up||If you start me up, I'll never stop||Never stop, never stop, never stop||You make a grown man cry||You make a grown man cry||You make a grown man cry||Spread out the oil, the gasoline||I walk smooth, ride in a mean, mean machine||Start it up||If you start it up||Kick on the starter, give it all you got||You got to, you got to||I can't compete with the riders in the other heats||If you rough it up||If you like it, I can slide it up||Slide it up, slide it up, slide it up||Don't make a grown man cry||Don't make a grown man cry||Don't make a grown man cry||My eyes dilate, my lips go green||My hands are greasy, she's a mean, mean machine||Start it up||Start me up||Ah, ah, give it all you've got||You've got to never, never, never stop||Slide it up, whoo!||Ah rev it up to start it up||Start it up, start it up, start it up||Never, never, never||You make a grown man cry||You make a grown man cry||You make a grown man cry||Ride like the wind at double speed||I'll take you places that you've never, never seen||Hey, hey||If you start it up||Love the day and we will never stop, never stop||Never, never, never stop||Start me up||Never stop, never stop||You, you, you make a grown man cry||You, you make a dead man cum||You, you make a dead man cum</t>
   </si>
   <si>
-    <t xml:space="preserve"> High Hopes</t>
-  </si>
-  <si>
     <t>Pray For The Wicked</t>
   </si>
   <si>
@@ -400,9 +322,6 @@
     <t>And disciplinary remains mercifully||Yes and um, I’m with you Derek, this star nonsense||Yes, yes, now which is it?||I am sure of it||So, so you think you can tell||Heaven from Hell? Blue skies from pain?||Can you tell a green field from a cold steel rail?||A smile from a veil? Do you think you can tell?||Did they get you to trade your heroes for ghosts?||Hot ashes for trees? Hot air for a cool breeze?||Cold comfort for change? Did you exchange||A walk-on part in the war for a lead role in a cage?||How I wish, how I wish you were here||We're just two lost souls swimming in a fishbowl, year after year||Running over the same old ground, what have we found?||The same old fears, wish you were here</t>
   </si>
   <si>
-    <t xml:space="preserve"> Is This Love</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bob Marley &amp; The Wailers </t>
   </si>
   <si>
@@ -412,12 +331,6 @@
     <t>I wanna love you||And treat you right||I wanna love you||Every day and every night||We'll be together||With a roof right over our heads||We'll share the shelter||Of my single bed||We'll share the same room, yeah||For Jah provide the bread||Is this love? Is this love? Is this love?||Is this love that I'm feeling?||Is this love? Is this love? Is this love?||Is this love that I'm feeling?||I wanna know, wanna know, wanna know now||I got to know, got to know, got to know now||I-I-I-I-I-I-I-I-I, I'm willing and able||So I throw my cards on your table||I wanna love you, I wanna love and treat||Love and treat you right||I wanna love you||Every day and every night||We'll be together, yeah||With a roof right over our heads||We'll share the shelter, yeah, oh-yeah||Of my single bed||We'll share the same room, yeah||For Jah provides the bread||Is this love? Is this love? Is this love?||Is this love that I'm feeling?||Is this love? Is this love? Is this love?||Is this love that I'm feeling?||Wo-o-o-oah||Oh, yes, I know; yes, I know, yes, I know now||Oh, yes, I know; yes, I know, yes, I know now||I-I-I-I-I-I-I-I-I, I'm willing and able||So I throw my cards on your table||See, I wanna love you, I wanna love and treat you||Love and treat you right||I wanna love you||Every day and every night||We'll be together||With a roof right over our heads||We'll share the shelter||Of my single bed||We'll share the same room, yeah||Jah provides the bread||We'll share the shelter||Of my single bed||We'll share the same room...</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sweet Child O' Mine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Guns N' Roses </t>
-  </si>
-  <si>
     <t>Appetite For Destruction</t>
   </si>
   <si>
@@ -433,9 +346,6 @@
     <t>Ooh-ooh, ooh-ooh, ooh-ooh, ooh||Ooh-ooh, ooh-ooh, ooh||Yeah, yeah, yeah (Ooh)||Baby, hit that back and burp||Then pour a four of purp'||You got his and hers||Toolie in that Birkin||Close the window curtains (Curtains)||Right up in your skirt (Skirt)||Take off, hit the curve (Curve)||Toolie in that Birkin||When I pop out, it's a blicky||We roll up, we roll up sticky||The other bitches, they be shifty||I pay for my shit, ain't shit free||Take some time (Hee, hee)||I know how I get when I make that mine||Shawty, I break that spine||Roll that dice||No covers, sex on ice (Yeah, yeah)||Ain't no lock and key||Just beep, beep, beep up in my Jeep||Baby, take off the belt of the seat||Touch-free, I brought somе ones||Shawty have fun with funds||Tongue out on camеra||Stretchin' out that Saint Laurent||She brought two friends, twin-twins||Casamigos killer||Fucked up off that liquor||Baby, hit that back and burp||Then pour a four of purp'||You got his and hers||Toolie in that Birkin||Close the window curtains (Curtains)||Right up in your skirt (Skirt)||Take off, hit the curve (Curve)||Toolie in that Birkin||When I pop out, it's a blicky||We roll up, we roll up sticky||The other bitches, they be shifty||I pay for my shit, ain't shit free||Take some time (Hee, hee)||I know how I get when I make that mine||Shawty, I break that spine||Toolie in that Birkin (Birkin)||You and me, I got you, that's for certain||We split a G6, it feel like surfin' (Surfin')||Talkin' to that big guy, trying to wash out my sins (Wash out my sins)||She was massaging me (Me), catered to a G (G)||I don't got to tell her about her body, she already got a physique (Physique)||Left from Croatia and landed in Greece (Greece)||I took her heart off her sleeve (Sleeve)||Love how you keep it a hundred, and that's really all that I need (That's all that I need, need)||I'm a big dog, and she on my turf||I just hope you know your worth||Baby, hit that back and burp||Baby, hit that back and burp||Then pour a four of purp'||You got his and hers||Toolie in that Birkin||Close the window curtains (Curtains)||Right up in your skirt (Skirt)||Take off, hit the curve (Curve)||Toolie in that Birkin||When I pop out, it's a blicky||We roll up, we roll up sticky||The other bitches, they be shifty||I pay for my shit, ain't shit free||Take some time (Hee, hee)||I know how I get when I make that mine||Shawty, I break that spine (Lil Uzi)||Huh, I know how I get (Yeah)||I'ma break your spine, next spot, I'm gon' break your ribs (Break your ribs, ayy)||Uh (Yeah), you know how I live (Yeah), so just cool out, baby (Cool out, baby)||I was born up in the nineties (Ayy), swag came from the eighties (Yeah, Lil Uzi)||I was sweatin' (Ayy), she on fire, we hot like it's Haiti (Ayy)||And you know I stay with bands on me like my name Katie (What?)||So much smoke coming out my blunt, it looked like I was vaping (Yeah)||I can't share none of my drugs (Ayy), know that I'm gon' face it (Yeah)||Any problem that I have, you know I'm gon' face it (Yeah)||Pop a Perky, Perc' in lean, and I barely taste it||Baby, hit that back and burp (Yeah)||Then pour a four of purp' (Lil Uzi)||You got his and hers||Toolie in that Birkin||Close the window curtains (Curtains)||Right up in your skirt (Skirt)||Take off, hit the curve (Curve)||Toolie in that Birkin||When I pop out, it's a blicky||We roll up, we roll up sticky||The other bitches, they be shifty||I pay for my shit, ain't shit free||Take some time (Hee, hee)||I know how I get when I make that mine||Shawty, I break that spine</t>
   </si>
   <si>
-    <t xml:space="preserve"> Borderline</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tame Impala </t>
   </si>
   <si>
@@ -445,9 +355,6 @@
     <t>Gone a little far||Gone a little far this time with something||How was I to know?||How was I to know this high came rushing?||We're on the borderline||Dangerously fine and unforgiven||Possibly a sign||I'm gonna have the strangest night on Sunday||Here I go||Quite a show for a loner in L.A.​||I wonder how I managed to end up in this place||Where I couldn't get away||We're on the borderline (Ooh)||Caught between the tides of pain and rapture||Then I saw the time||Watched it speedin' by like a train||Like a train||Will I be known and loved?||Is there one that I trust?||Starting to sober up||Has it been long enough?||Will I be known and loved?||Little closer, close enough||I'm a loser, loosen up||Setting free, must be tough||Will I be known and loved?||Is there one that I trust?||Starting to sober up||Has it been long enough?||Will I be so in love?||Any closer? Close enough||Shout out to what is done||R.I.P., here comes the sun||(Comes the sun)||Gone a little far||Gone a little far this time with something||Rudi said it's fine||They used to do this all the time in college (If you and I get comfortable)||And we're on the borderline (Ooh)||Caught between the tides of pain and rapture||Then I saw the time||Watched it speedin' by like a train||Will I be known and loved?||Is there one that I trust?||Starting to sober up||Has it been long enough?||Will I be known and loved?||Little closer, close enough||I'm a loser, loosen up||Setting free, must be tough||Will I be known and loved?||Is there one that I trust?||Starting to sober up||Has it been long enough?||Will I be so in love?||Any closer? Close enough||Shout out to what is done||R.I.P., here comes the sun||(Comes the sun)</t>
   </si>
   <si>
-    <t xml:space="preserve"> One More Time</t>
-  </si>
-  <si>
     <t xml:space="preserve">Daft Punk </t>
   </si>
   <si>
@@ -457,9 +364,6 @@
     <t>One more time||One more time||One more time||We're gonna celebrate||Oh yeah, all right||Don't stop the dancing||One more time||We're gonna celebrate||Oh yeah, all right||Don't stop the dancing||One more time||We're gonna celebrate||Oh yeah, all right||Don't stop the dancing||One more time||We're gonna celebrate||Oh yeah||One more time||One more time||We're gonna celebrate||Oh yeah, all right||Don't stop the dancing||One more time||We're gonna celebrate||Oh yeah||Don't stop the dancing||One more time||Mmm, you know I'm just feeling||Celebration tonight||Celebrate||Don't wait too late||Mmm, no||We don't stop||You can't stop||We're gonna celebrate||One more time||One more time||One more time||A celebration||You know we're gonna do it right, tonight||Hey! Just feeling||Music's got me feeling the need||Need, yeah||Come on, all right||We're gonna celebrate||One more time||Celebrate and dance so free||Music's got me feeling so free||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate||One more time||Music's got me feeling so free||We're gonna celebrate||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate||Celebrate and dance so free||One more time||Music's got me feeling so free||We're gonna celebrate</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sucker</t>
-  </si>
-  <si>
     <t xml:space="preserve">Jonas Brothers </t>
   </si>
   <si>
@@ -469,18 +373,12 @@
     <t>We go together||Better than birds of a feather, you and me||We change the weather, yeah||I'm feelin' heat in December when you're 'round me||I've been dancin' on top of cars and stumblin' out of bars||I follow you through the dark, can't get enough||You're the medicine and the pain, the tattoo inside my brain||And, baby, you know it's obvious||I'm a sucker for you||You say the word and I'll go anywhere blindly||I'm a sucker for you, yeah||Any road you take, you know that you'll find me||I'm a sucker for all the subliminal things||No one knows about you (About you), about you (About you)||And you're makin' the typical me break my typical rules||It's true, I'm a sucker for you, yeah||Don't complicate it (Yeah)||'Cause I know you and you know everything about me||I can't remember (Yeah) all of the nights||I don't remember when you're 'round me (Oh, yeah, yeah)||I've been dancin' on top of cars and stumblin' out of bars||I follow you through the dark, can't get enough||You're the medicine and the pain, the tattoo inside my brain||And, baby, you know it's obvious||I'm a sucker for you||You say the word and I'll go anywhere blindly||I'm a sucker for you, yeah||Any road you take, you know that you'll find me||I'm a sucker for all the subliminal things||No one knows about you (About you), about you (About you)||And you're makin' the typical me break my typical rules||It's true, I'm a sucker for you, yeah (Uh)||(I'm a sucker for you)||I've been dancin' on top of cars and stumblin' out of bars||I follow you through the dark, can't get enough||You're the medicine and the pain, the tattoo inside my brain||And, baby, you know it's obvious||I'm a sucker for you, yeah||Say the word and I'll go anywhere blindly||I'm a sucker for you, yeah||Any road you take, you know that you'll find me||I'm a sucker for all the subliminal things||No one knows about you (About you), about you (About you)||And you're makin' the typical me break my typical rules||It's true, I'm a sucker for you (Uh)||I'm a sucker for you</t>
   </si>
   <si>
-    <t xml:space="preserve"> Beautiful Day</t>
-  </si>
-  <si>
     <t>All That You Can't Leave Behind</t>
   </si>
   <si>
     <t>The heart is a bloom, shoots up through the stony ground||There's no room, no space to rent in this town||You're out of luck, and the reason that you had to care||The traffic is stuck, and you're not moving anywhere||You thought you'd found a friend to take you out of this place||Someone you could lend a hand in return for grace||It's a beautiful day||Sky falls, you feel like||It's a beautiful day||Don't let it get away||You're on the road, but you've got no destination||You're in the mud, in the maze of her imagination||You love this town even if that doesn't ring true||You've been all over, and it's been all over you||It's a beautiful day||Don't let it get away||It's a beautiful day||Ooh-hoo-hoo||Touch me||Take me to that other place||Teach me||I know I'm not a hopeless case||See the world in green and blue||See China right in front of you||See the canyons broken by cloud||See the tuna fleets clearing the sea out||See the Bedouin fires at night||See the oil fields at first light||And see the bird with a leaf in her mouth||After the flood all the colours came out||It was a beautiful day||Don't let it get away||Beautiful day||Touch me||Take me to that other place||Reach me||I know I'm not a hopeless case||What you don't have you don't need it now||What you don't know you can feel it somehow||What you don't have you don't need it now||Don't need it now||Was a beautiful day</t>
   </si>
   <si>
-    <t xml:space="preserve"> It's My Life</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bon Jovi </t>
   </si>
   <si>
@@ -541,9 +439,6 @@
     <t>As the snow flies||On a cold and gray Chicago mornin'||A poor little baby child is born||In the ghetto (In the ghetto)||And his mama cries||'Cause if there's one thing that she don't need||It's another hungry mouth to feed||In the ghetto (In the ghetto)||People, don't you understand||A child needs a helping hand||Or he'll grow to be an angry young man some day||Take a look at you and me||Are we too blind to see||Do we simply turn our heads||And look the other way?||Well, the world turns||And a hungry little boy with a runny nose||Plays in the street as the cold wind blows||In the ghetto (In the ghetto)||And his hunger burnsSo he starts to roam the streets at night||And he learns how to steal and he learns how to fight||In the ghetto (In the ghetto)||Then one night in desperation||The young man breaks away||He buys a gun, he steals a car||Tries to run, but he don't get far||And his mama cries||As a crowd gathers 'round an angry young man||Facedown on the street with a gun in his hand||In the ghetto (In the ghetto)||And as her young man dies (In the ghetto)||On a cold and gray Chicago mornin'||Another little baby child is born||In the ghetto (In the ghetto)||And his mama cries||In the ghetto (In the ghetto)||(In the ghetto)</t>
   </si>
   <si>
-    <t>Johnny B.Goode</t>
-  </si>
-  <si>
     <t>Chuck Berry</t>
   </si>
   <si>
@@ -604,9 +499,6 @@
     <t>I don't want you be no slave||I don't want you work all day||I don't want 'cause I'm sad and blue||I just want to make love to you, baby||Love to you, baby||Love to you, baby||Love to you||I don't want you cook my bread||I don't t want you make my bed||I don't want your money too||I just want to make love to you, baby||Love to you, baby||Love to you, baby||Love to you||Well I can tell by the way that you twitch and walk||See by the way that you baby talk||Know by the way that you treat your man||I can love you, baby, till the cryin' shame||I don't want you wash my clothes||I don't want you leave the home||I don't want 'cause I'm sad and blue||I just want to make love to you, baby||Love to you, baby||Love to you, baby||Love to you||I don't want you wash my clothes||I don't want you leave the home||I don't want 'cause I'm sad and blue||I just want to make love to you, baby||Love to you, baby||Love to you, baby||Sweet love to you, baby||Love to you, baby||I just want to make love to you, baby||Love to you, baby||Love to you, baby||Love to you||I just, I just want to make love to you, baby||I just want to make</t>
   </si>
   <si>
-    <t>Ain't That A Shame</t>
-  </si>
-  <si>
     <t>Fats Domino</t>
   </si>
   <si>
@@ -616,9 +508,6 @@
     <t>You made me cry||When you said goodbye||Ain't that a shame?||My tears fell like rain||Ain't that a shame?||You're the one to blame||You broke my heart||When you said we'll part||Ain't that a shame?||My tears fell like rain||Ain't that a shame?||You're the one to blame||Oh, well, goodbye||Although I'll cry||Ain't that a shame?||My tears fell like rain||Ain't that a shame?||You're the one to blame||You made me cry||When you said goodbye||Ain't that a shame?||My tears fell like rain||Ain't that a shame?||You're the one to blame||Oh well, goodbye||Although I'll cry||Ain't that a shame?||My tears fell like rain||Ain't that a shame?||You're the one to blame</t>
   </si>
   <si>
-    <t>That' All</t>
-  </si>
-  <si>
     <t>My Man And I / That's All</t>
   </si>
   <si>
@@ -655,18 +544,12 @@
     <t>The warden threw a party in the county jail||The prison band was there and they began to wail||The band was jumping and the joint began to swing||You shoulda heard those knocked out jailbirds sing||Let's rock, everybody, let's rock||Everybody in the whole cell block||Was dancing to the Jailhouse Rock||Spider Murphy played the tenor saxophone||Little Joey blowing on the slide trombone||The drummer boy from Illinois went crash, boom, bang||The whole rhythm section was the Purple Gang||Let's rock, everybody, let's rock||Everybody in the whole cell block||Was dancing to the Jailhouse Rock||Number forty-seven said to number three||"You the cutest jailbird I ever did see||I sure would be delighted with your company||Come on and do the Jailhouse Rock with me"||Let's rock, everybody, let's rock||Everybody in the whole cell block||Was dancing to the Jailhouse Rock||Rock, rock, rock||Sad Sack was sitting on a block of stone||Way over in the corner weeping all alone||The warden said, "Hey, buddy, don't you be no square||You can't find a partner, use a wooden chair"||Let's rock, everybody, let's rock||Everybody in the whole cell block||Was dancing to the Jailhouse Rock||Shifty Henry said to Bugs, "For Heaven's sake||No one's looking, now's our chance to make a break"||Bugsy turned to Shifty and he said, "Nix nix||I wanna stick around a while and get my kicks."||Let's rock, everybody, let's rock||Everybody in the whole cell block||Was dancing to the Jailhouse Rock||Dancing to the Jailhouse Rock||Dancing to the Jailhouse Rock||Dancing to the Jailhouse Rock||Dancing to the Jailhouse Rock</t>
   </si>
   <si>
-    <t>Jumpin' Jack Flash</t>
-  </si>
-  <si>
     <t>Through the Past, Darkly (Big Hits Vol. 2)</t>
   </si>
   <si>
     <t>Watch it!||I was born in a crossfire hurricane||And I howled at my ma in the drivin' rain||But it's all right now||In fact, it's a gas||But it's all right||I'm Jumpin' Jack Flash||It's a gas, gas, gas||I was raised by a toothless, bearded hag||I was schooled with a strap right across my back||But it's all right now||In fact, it's a gas||But it's all right||I'm Jumpin' Jack Flash||It's a gas, gas, gas||Ooh!||I was drowned, I was washed up and left for dead||I fell down to my feet and I saw they bled, yeah, yeah||I frowned at the crumbs of a crust of bread, yeah, yeah||I was crowned with a spike right through my head||My, my, yeah||But it's all right now||In fact, it's a gas||But it's all right||I'm Jumpin' Jack Flash||It's a gas, gas, gas||Jumpin' Jack Flash, it's a gas||Jumpin' Jack Flash, it's a gas||Jumpin' Jack Flash, it's a gas||Jumpin' Jack Flash, it's a gas||Jumpin' Jack Flash, it's a gas||Jumpin' Jack Flash, it's a gas</t>
   </si>
   <si>
-    <t>Oh, Pretty Woman</t>
-  </si>
-  <si>
     <t>Roy Orbison</t>
   </si>
   <si>
@@ -778,18 +661,12 @@
     <t>Out of all the reindeers, you know you're the mastermind||Run, run, Rudolph, Randolph ain't too far behind||Run, run, Rudolph, Santa's got to make it to town||Santa make him hurry, tell him he can take the freeway down||Run, run, Rudolph cause I'm reeling like a merry-go-round||Said Santa to a boy, "Child, what have you been longing for?"||"All I want for Christmas is a rock and roll electric guitar"||And then away went Rudolph whizzing like a shooting star||Run, run, Rudolph, Santa has to make it to town||Santa make him hurry, tell him he can take the freeway down||Run, run, Rudolph, reeling like a merry-go-round||Run, run, Rudolph, Santa's got to make it to town||Santa make him hurry, tell him he can take the freeway down||Run, run, Rudolph, I'm reeling like a merry-go-round||Said Santa to a girl, "Child, what would please you most to get?"||"A little baby doll that can cry, sleep, drink, and wet"||And then away went Rudolph, whizzing like a Sabre jet||Run, run, Rudolph, Santa's got to make it to town||Santa make him hurry, tell him he can take the freeway down||Run, run, Rudolph, I'm reeling like a merry-go-round</t>
   </si>
   <si>
-    <t>Whole Lot Of Shakin' Going On</t>
-  </si>
-  <si>
     <t>The Golden Hits of Jerry Lee Lewis</t>
   </si>
   <si>
     <t>Well, come on over baby||Whole lot of shakin' goin' on||I said come on over baby||Baby, you can't go wrong||We ain't fakin'||Whole lotta shakin' goin' on||Well, I said come on over baby||We got chicken in the barn, woo-a||Come on over baby||Really got the bull by the horn||We ain't fakin'||Whole lotta shakin' goin' on||Well, I said shake baby, shake it||I said shake baby, shake it||I said shake it baby, shake it||I said shake baby, shake||Come on over||Whole lotta shakin' goin' on||Ah, let's go||Come on over baby||We got chicken in the barn||Whose barn, what barn, my barn||Come on over baby really got the bull by the horn||We ain't fakin' whole lot of shakin' going on||Easy now||Shake||Well, shake it baby, yeah||You can shake one time for me||Come over baby||Whole lot of shakin' goin' on||Now real low one time now||Shake baby shake||All you gotta do honey||Is kinda stand in one tight little spot||And wiggle around just a little bit||And that's when you got something yeah||Well you got to shake it for me||Now let's go one time||||Shake it baby, shake it||Shake it baby, shake, ooo||Come on baby||Shake, baby shake it||Come on overWhole lotta shakin' goin' on</t>
   </si>
   <si>
-    <t>I'm A King Bee</t>
-  </si>
-  <si>
     <t>Well I'm a king bee buzzing around your hive||Well I'm a king bee, baby, buzzing around your hive||Yeah I can make honey baby, let me come inside||Well I'm a king bee, want you to be my queen||Well I'm a king bee, baby, want you to be my queen||Together we can make honey the world has never seen||Well, buzz a while||Sting you bad||Well I'm a king bee, can buzz all night long||Well I'm a king bee, baby, can buzz all night long||Yeah I can buzz better baby when your man is gone</t>
   </si>
   <si>
@@ -898,9 +775,6 @@
     <t>To do do, down dooby doo down down||Comma comma, down dooby doo down down||Comma comma, down dooby doo down down||Breaking up is hard to do||Don't take your love away from me!||Don't you leave my heart in misery?||If you go, then I'll be blue!||'Cuz breaking up is hard to do||Remember when you held me tight||And you kissed me all through the night||Think of all that we've been through||And breaking up is hard to do||They say that breaking up is hard to do||Now, I know, I know that it's true!||Don't say that this is the end!||Instead of breaking up, I wish we were making up again||I beg of you, don't say goodbye!||Can't we give our love another try?||Come on, baby, let's start a new!||'Cuz breaking up is hard to do||They say that breaking up is hard to do||Now, I know, I know that it's true!||Don't say that this is the end!||Instead of breaking up, I wish we were making up again||I beg of you, don't say goodbye!||Can't we give our love another try?||Come on, baby, let's start a new!||'Cuz breaking up is hard to do||To do do, down dooby doo down down||Comma comma, down dooby doo down down||Comma comma, down dooby doo down down||Comma comma, down dooby doo down down||Comma comma</t>
   </si>
   <si>
-    <t>Boppin' The Blues</t>
-  </si>
-  <si>
     <t>Well, all my friends are boppin' the blues; it must be goin' round||All my friends are boppin' the blues; it must be goin' roundI love you, baby, but I must be rhythm bound||Well, the doctor told me, Carl you need no pills||Yes, the doctor told me, boy, you don't need no pills||Just a handful of nickels, the juke box will cure your ills||Well, all my friends are boppin' the blues; it must be goin' round||All them cats are boppin' the blues; it must be goin' round||I love you, baby, but I must be rhythm bound||Well, the old cat bug bit me, man, I don't feel no pain||Yeah, that jitterbug caught me, man, I don't feel no pain||I still love you baby, but I'll never be the same||I said, all my friends are boppin' the blues; it must be goin' round||All my friends are boppin' the blues; it must be goin' round||I love you, baby, but I must be rhythm bound||Well, all my friends are boppin' the blues; it must be goin' round||All them cats are boppin' the blues; it must be goin' round||I love you, baby, but I must be rhythm bound||Well, grand-pa Don got rhythm and he threw his crutches down||Oh the old boy Don got rhythm and blues and he threw that crutches down||Grand-ma, he ain't triflin', well the old boy's rhythm bound||Well, all them cats are boppin' the blues; it must be goin' round||All my friends are boppin' the blues; it must be goin' round||I love you, baby, but I must be rhythm bound||A rock bop, rhythm and blues||A rock bop, rhythm and blues||A rock rock, rhythm and blues||A rock rock, rhythm and blues||Rhythm and blues, it must be goin' round</t>
   </si>
   <si>
@@ -1081,36 +955,15 @@
     <t>Maneskin</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ice Cream</t>
-  </si>
-  <si>
     <t>The Chainsmokers</t>
   </si>
   <si>
-    <t xml:space="preserve"> Start Me Up</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wish You Were Here</t>
-  </si>
-  <si>
     <t xml:space="preserve">Panic At The Disco </t>
   </si>
   <si>
-    <t xml:space="preserve"> His &amp; Hers</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Whole Lotta Love</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Let It Be</t>
-  </si>
-  <si>
     <t>Twist And Shout</t>
   </si>
   <si>
-    <t>Shout, Sister, Shout</t>
-  </si>
-  <si>
     <t xml:space="preserve">All My Loving </t>
   </si>
   <si>
@@ -1123,27 +976,18 @@
     <t>Folsom Prison Blues</t>
   </si>
   <si>
-    <t xml:space="preserve">Surfin' U.S.A. </t>
-  </si>
-  <si>
     <t>I Saw Her Standing There</t>
   </si>
   <si>
     <t>All Your Love</t>
   </si>
   <si>
-    <t>A Hard Day's Night</t>
-  </si>
-  <si>
     <t>2U</t>
   </si>
   <si>
     <t>Blackpink</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
     <t>Another One Bites The Dust</t>
   </si>
   <si>
@@ -1196,6 +1040,156 @@
   </si>
   <si>
     <t>All the single ladies (All the single ladies)||All the single ladies (All the single ladies)||All the single ladies (All the single ladies)||All the single ladies||Now put your hands up||Up in the club (club), just broke up (up)||I’m doing my own little thing||Decided to dip (dip), but now you wanna trip (trip)||'Cause another brother noticed me||I’m up on him (him), he up on me (me)||Don’t pay him any attention||Cried my tears (tears), for three good years (years)||You can’t be mad at me||'Cause if you like it, then you shoulda put a ring on it||If you like it, then you shoulda put a ring on it||Don’t be mad once you see that he want it||If you like it, then you shoulda put a ring on it||Whoa, oh, oh, oh, oh-oh, oh, oh, oh, oh, oh, oh||Whoa, oh, oh, oh, oh-oh, oh, oh, oh, oh, oh, oh||'Cause if you like it, then you shoulda put a ring on it||If you like it, then you shoulda put a ring on it||Don’t be mad once you see that he want it||If you like it, then you shoulda put a ring on it||I got gloss on my lips (lips), a man on my hips (hips)||Hold me tighter than my Deréon jeans||Acting up (up), drink in my cup (cup)||I can't care less what you think||I need no permission, did I mention?||Don’t pay him any attention||'Cause you had your turn (turn)||But now you gon' learn||What it really feels like to miss me||'Cause if you like it, then you shoulda put a ring on it||If you like it, then you shoulda put a ring on it||Don’t be mad once you see that he want it||If you like it, then you shoulda put a ring on it||Whoa, oh, oh, oh, oh-oh, oh, oh, oh, oh, oh, oh||Whoa, oh, oh, oh, oh-oh, oh, oh, oh, oh, oh, oh||'Cause if you like it, then you shoulda put a ring on it||If you like it, then you shoulda put a ring on it||Don’t be mad once you see that he want it||If you like it, then you shoulda put a ring on it||Whoa, oh, oh, oh, oh-oh, oh, oh, oh, oh, oh, oh||Whoa, oh, oh, oh, oh-oh, oh, oh, oh, oh, oh, oh||Don't treat me to the things of the world||I’m not that kind of girl||Your love is what I prefer, what I deserve||Here’s a man that makes me, then takes me||And delivers me to a destiny, to infinity and beyond||Pull me into your arms||Say I’m the one you want||If you don’t, you’ll be alone||And like a ghost, I’ll be gone||All the single ladies (All the single ladies)||All the single ladies (All the single ladies)||All the single ladies (All the single ladies)||All the single ladies||Now put your hands up||Whoa, oh, oh, oh, oh-oh, oh, oh, oh, oh, oh, oh||Whoa, oh, oh, oh, oh-oh, oh, oh, oh, oh, oh, oh||Whoa, oh, oh, oh||'Cause if you like it, then you shoulda put a ring on it||If you like it, then you shoulda put a ring on it||Don’t be mad once you see that he want it||If you like it, then you shoulda put a ring on it||Whoa, oh, oh, oh||'Cause if you like it, then you shoulda put a ring on it||If you like it, then you shoulda put a ring on it||Don’t be mad once you see that he want it||If you like it, then you shoulda put a ring on it||Whoa, oh, oh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC DC </t>
+  </si>
+  <si>
+    <t>Maroon Five</t>
+  </si>
+  <si>
+    <t>U Two</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Five Seconds of Summer </t>
+  </si>
+  <si>
+    <t>Abba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guns N Roses </t>
+  </si>
+  <si>
+    <t>Johnny B Goode</t>
+  </si>
+  <si>
+    <t>Ain t That A Shame</t>
+  </si>
+  <si>
+    <t>Jumpin Jack Flash</t>
+  </si>
+  <si>
+    <t>Oh Pretty Woman</t>
+  </si>
+  <si>
+    <t>Whole Lot Of Shakin Going On</t>
+  </si>
+  <si>
+    <t>That ll Be The Day</t>
+  </si>
+  <si>
+    <t>Shout Sister Shout</t>
+  </si>
+  <si>
+    <t>I m A King Bee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surfin USA </t>
+  </si>
+  <si>
+    <t>Boppin The Blues</t>
+  </si>
+  <si>
+    <t>A Hard Days Night</t>
+  </si>
+  <si>
+    <t>That All</t>
+  </si>
+  <si>
+    <t>Follow You</t>
+  </si>
+  <si>
+    <t>Best Song Ever</t>
+  </si>
+  <si>
+    <t>Let It Be</t>
+  </si>
+  <si>
+    <t>Beggin</t>
+  </si>
+  <si>
+    <t>Why d You Only Call Me When You're High</t>
+  </si>
+  <si>
+    <t>In the End</t>
+  </si>
+  <si>
+    <t>Ice Cream</t>
+  </si>
+  <si>
+    <t>Shy Away</t>
+  </si>
+  <si>
+    <t>Sweater Weather</t>
+  </si>
+  <si>
+    <t>Scar Tissue</t>
+  </si>
+  <si>
+    <t>Thunderstruck</t>
+  </si>
+  <si>
+    <t>I Gotta Feeling</t>
+  </si>
+  <si>
+    <t>Someday</t>
+  </si>
+  <si>
+    <t>Enter Sandman</t>
+  </si>
+  <si>
+    <t>Sweet Melody</t>
+  </si>
+  <si>
+    <t>Takeaway</t>
+  </si>
+  <si>
+    <t>Heat Waves</t>
+  </si>
+  <si>
+    <t>Come As You Are</t>
+  </si>
+  <si>
+    <t>Straightenin</t>
+  </si>
+  <si>
+    <t>Boulevard of Broken Dreams</t>
+  </si>
+  <si>
+    <t>Chiquitita</t>
+  </si>
+  <si>
+    <t>Start Me Up</t>
+  </si>
+  <si>
+    <t>High Hopes</t>
+  </si>
+  <si>
+    <t>Wish You Were Here</t>
+  </si>
+  <si>
+    <t>Is This Love</t>
+  </si>
+  <si>
+    <t>Sweet Child O Mine</t>
+  </si>
+  <si>
+    <t>Borderline</t>
+  </si>
+  <si>
+    <t>One More Time</t>
+  </si>
+  <si>
+    <t>Sucker</t>
+  </si>
+  <si>
+    <t>Beautiful Day</t>
+  </si>
+  <si>
+    <t>It s My Life</t>
+  </si>
+  <si>
+    <t>Whole Lotta Love</t>
   </si>
 </sst>
 </file>
@@ -1273,6 +1267,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1565,8 +1563,8 @@
   </sheetPr>
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,41 +1678,41 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" t="s">
         <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>358</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>31</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>359</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
         <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1722,1442 +1720,1442 @@
         <v>360</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>361</v>
       </c>
       <c r="B12" t="s">
-        <v>352</v>
+        <v>310</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>362</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>363</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="B15" t="s">
-        <v>372</v>
+        <v>321</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>365</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>366</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>367</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>368</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>340</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>369</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>370</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>371</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>372</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>373</v>
       </c>
       <c r="B24" t="s">
-        <v>354</v>
+        <v>311</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>374</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>375</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="D27" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>376</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>377</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="D29" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>343</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>378</v>
       </c>
       <c r="B31" t="s">
-        <v>114</v>
+        <v>344</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>355</v>
+        <v>379</v>
       </c>
       <c r="B32" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>120</v>
+        <v>380</v>
       </c>
       <c r="B33" t="s">
-        <v>357</v>
+        <v>312</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="D33" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>356</v>
+        <v>381</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="D34" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>382</v>
       </c>
       <c r="B35" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
       <c r="D35" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>383</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>345</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="D36" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>358</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
       <c r="D37" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>137</v>
+        <v>384</v>
       </c>
       <c r="B38" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
       <c r="D38" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>141</v>
+        <v>385</v>
       </c>
       <c r="B39" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="D39" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>145</v>
+        <v>386</v>
       </c>
       <c r="B40" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
       <c r="D40" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>387</v>
       </c>
       <c r="B41" t="s">
-        <v>373</v>
+        <v>342</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="D41" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>152</v>
+        <v>388</v>
       </c>
       <c r="B42" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="D42" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>359</v>
+        <v>389</v>
       </c>
       <c r="B43" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="D43" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
       <c r="B44" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="D44" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="B45" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="D45" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="B46" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="D46" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="B47" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="D47" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>173</v>
+        <v>346</v>
       </c>
       <c r="B48" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="D48" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="B49" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="D49" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="B50" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="D50" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="B51" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="D51" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>152</v>
       </c>
       <c r="B52" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>189</v>
+        <v>154</v>
       </c>
       <c r="D52" t="s">
-        <v>190</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="D53" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>194</v>
+        <v>347</v>
       </c>
       <c r="B54" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="D54" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>198</v>
+        <v>357</v>
       </c>
       <c r="B55" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>199</v>
+        <v>162</v>
       </c>
       <c r="D55" t="s">
-        <v>200</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>164</v>
       </c>
       <c r="B56" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>203</v>
+        <v>166</v>
       </c>
       <c r="D56" t="s">
-        <v>204</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="B57" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>207</v>
+        <v>170</v>
       </c>
       <c r="D57" t="s">
-        <v>208</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="B58" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>209</v>
+        <v>172</v>
       </c>
       <c r="D58" t="s">
-        <v>210</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>211</v>
+        <v>348</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="D59" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>214</v>
+        <v>349</v>
       </c>
       <c r="B60" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>216</v>
+        <v>177</v>
       </c>
       <c r="D60" t="s">
-        <v>217</v>
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>361</v>
+        <v>313</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>218</v>
+        <v>179</v>
       </c>
       <c r="D61" t="s">
-        <v>219</v>
+        <v>180</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>220</v>
+        <v>181</v>
       </c>
       <c r="B62" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="D62" t="s">
-        <v>221</v>
+        <v>182</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>222</v>
+        <v>183</v>
       </c>
       <c r="B63" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="D63" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="B64" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>185</v>
+        <v>150</v>
       </c>
       <c r="D64" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="B65" t="s">
-        <v>227</v>
+        <v>188</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>228</v>
+        <v>189</v>
       </c>
       <c r="D65" t="s">
-        <v>229</v>
+        <v>190</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>230</v>
+        <v>191</v>
       </c>
       <c r="B66" t="s">
-        <v>231</v>
+        <v>192</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>232</v>
+        <v>193</v>
       </c>
       <c r="D66" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>234</v>
+        <v>195</v>
       </c>
       <c r="B67" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
       <c r="D67" t="s">
-        <v>235</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="B68" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="D68" t="s">
-        <v>239</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="B69" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>240</v>
+        <v>201</v>
       </c>
       <c r="D69" t="s">
-        <v>241</v>
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>242</v>
+        <v>351</v>
       </c>
       <c r="B70" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>242</v>
+        <v>203</v>
       </c>
       <c r="D70" t="s">
-        <v>244</v>
+        <v>205</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>245</v>
+        <v>206</v>
       </c>
       <c r="B71" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>246</v>
+        <v>207</v>
       </c>
       <c r="D71" t="s">
-        <v>247</v>
+        <v>208</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>363</v>
+        <v>314</v>
       </c>
       <c r="B72" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>248</v>
+        <v>209</v>
       </c>
       <c r="D72" t="s">
-        <v>249</v>
+        <v>210</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>364</v>
+        <v>315</v>
       </c>
       <c r="B73" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>250</v>
+        <v>211</v>
       </c>
       <c r="D73" t="s">
-        <v>251</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>252</v>
+        <v>350</v>
       </c>
       <c r="B74" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>253</v>
+        <v>213</v>
       </c>
       <c r="D74" t="s">
-        <v>254</v>
+        <v>214</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>255</v>
+        <v>353</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>192</v>
+        <v>157</v>
       </c>
       <c r="D75" t="s">
-        <v>256</v>
+        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>365</v>
+        <v>316</v>
       </c>
       <c r="B76" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>257</v>
+        <v>216</v>
       </c>
       <c r="D76" t="s">
-        <v>258</v>
+        <v>217</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>259</v>
+        <v>218</v>
       </c>
       <c r="B77" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>260</v>
+        <v>219</v>
       </c>
       <c r="D77" t="s">
-        <v>261</v>
+        <v>220</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>366</v>
+        <v>317</v>
       </c>
       <c r="B78" t="s">
-        <v>188</v>
+        <v>153</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>262</v>
+        <v>221</v>
       </c>
       <c r="D78" t="s">
-        <v>263</v>
+        <v>222</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="B79" t="s">
-        <v>264</v>
+        <v>223</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>265</v>
+        <v>224</v>
       </c>
       <c r="D79" t="s">
-        <v>266</v>
+        <v>225</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>267</v>
+        <v>226</v>
       </c>
       <c r="B80" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>268</v>
+        <v>227</v>
       </c>
       <c r="D80" t="s">
-        <v>269</v>
+        <v>228</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>270</v>
+        <v>229</v>
       </c>
       <c r="B81" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>268</v>
+        <v>227</v>
       </c>
       <c r="D81" t="s">
-        <v>271</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="B82" t="s">
-        <v>272</v>
+        <v>231</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>273</v>
+        <v>232</v>
       </c>
       <c r="D82" t="s">
-        <v>274</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>275</v>
+        <v>234</v>
       </c>
       <c r="B83" t="s">
-        <v>272</v>
+        <v>231</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>273</v>
+        <v>232</v>
       </c>
       <c r="D83" t="s">
-        <v>276</v>
+        <v>235</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>277</v>
+        <v>236</v>
       </c>
       <c r="B84" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>278</v>
+        <v>237</v>
       </c>
       <c r="D84" t="s">
-        <v>279</v>
+        <v>238</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>280</v>
+        <v>239</v>
       </c>
       <c r="B85" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>281</v>
+        <v>240</v>
       </c>
       <c r="D85" t="s">
-        <v>282</v>
+        <v>241</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>283</v>
+        <v>242</v>
       </c>
       <c r="B86" t="s">
-        <v>202</v>
+        <v>165</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>284</v>
+        <v>243</v>
       </c>
       <c r="D86" t="s">
-        <v>285</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>286</v>
+        <v>245</v>
       </c>
       <c r="B87" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>260</v>
+        <v>219</v>
       </c>
       <c r="D87" t="s">
-        <v>287</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>368</v>
+        <v>318</v>
       </c>
       <c r="B88" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>218</v>
+        <v>179</v>
       </c>
       <c r="D88" t="s">
-        <v>288</v>
+        <v>247</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>289</v>
+        <v>248</v>
       </c>
       <c r="B89" t="s">
-        <v>231</v>
+        <v>192</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>290</v>
+        <v>249</v>
       </c>
       <c r="D89" t="s">
-        <v>291</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>292</v>
+        <v>355</v>
       </c>
       <c r="B90" t="s">
-        <v>272</v>
+        <v>231</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>273</v>
+        <v>232</v>
       </c>
       <c r="D90" t="s">
-        <v>293</v>
+        <v>251</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="B91" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="D91" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>296</v>
+        <v>254</v>
       </c>
       <c r="B92" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>297</v>
+        <v>255</v>
       </c>
       <c r="D92" t="s">
-        <v>298</v>
+        <v>256</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>369</v>
+        <v>319</v>
       </c>
       <c r="B93" t="s">
-        <v>299</v>
+        <v>257</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>300</v>
+        <v>258</v>
       </c>
       <c r="D93" t="s">
-        <v>301</v>
+        <v>259</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>370</v>
+        <v>356</v>
       </c>
       <c r="B94" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>302</v>
+        <v>260</v>
       </c>
       <c r="D94" t="s">
-        <v>303</v>
+        <v>261</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>304</v>
+        <v>262</v>
       </c>
       <c r="B95" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>305</v>
+        <v>263</v>
       </c>
       <c r="D95" t="s">
-        <v>306</v>
+        <v>264</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>307</v>
+        <v>265</v>
       </c>
       <c r="B96" t="s">
-        <v>308</v>
+        <v>266</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>309</v>
+        <v>267</v>
       </c>
       <c r="D96" t="s">
-        <v>310</v>
+        <v>268</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>311</v>
+        <v>269</v>
       </c>
       <c r="B97" t="s">
-        <v>312</v>
+        <v>270</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>313</v>
+        <v>271</v>
       </c>
       <c r="D97" t="s">
-        <v>314</v>
+        <v>272</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>315</v>
+        <v>273</v>
       </c>
       <c r="B98" t="s">
-        <v>316</v>
+        <v>274</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>317</v>
+        <v>275</v>
       </c>
       <c r="D98" t="s">
-        <v>318</v>
+        <v>276</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>319</v>
+        <v>277</v>
       </c>
       <c r="B99" t="s">
-        <v>320</v>
+        <v>278</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>321</v>
+        <v>279</v>
       </c>
       <c r="D99" t="s">
-        <v>322</v>
+        <v>280</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>323</v>
+        <v>281</v>
       </c>
       <c r="B100" t="s">
-        <v>324</v>
+        <v>282</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>325</v>
+        <v>283</v>
       </c>
       <c r="D100" t="s">
-        <v>326</v>
+        <v>284</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>371</v>
+        <v>320</v>
       </c>
       <c r="B101" t="s">
-        <v>327</v>
+        <v>285</v>
       </c>
       <c r="C101" s="2">
         <v>7</v>
       </c>
       <c r="D101" t="s">
-        <v>328</v>
+        <v>286</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>329</v>
+        <v>287</v>
       </c>
       <c r="B102" t="s">
-        <v>330</v>
+        <v>288</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>330</v>
+        <v>288</v>
       </c>
       <c r="D102" t="s">
-        <v>331</v>
+        <v>289</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>332</v>
+        <v>290</v>
       </c>
       <c r="B103" t="s">
-        <v>333</v>
+        <v>291</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>334</v>
+        <v>292</v>
       </c>
       <c r="D103" t="s">
-        <v>335</v>
+        <v>293</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>336</v>
+        <v>294</v>
       </c>
       <c r="B104" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>337</v>
+        <v>295</v>
       </c>
       <c r="D104" t="s">
-        <v>338</v>
+        <v>296</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>339</v>
+        <v>297</v>
       </c>
       <c r="B105" t="s">
-        <v>340</v>
+        <v>298</v>
       </c>
       <c r="C105" s="2">
         <v>21</v>
       </c>
       <c r="D105" t="s">
-        <v>341</v>
+        <v>299</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>342</v>
+        <v>300</v>
       </c>
       <c r="B106" t="s">
-        <v>333</v>
+        <v>291</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>342</v>
+        <v>300</v>
       </c>
       <c r="D106" t="s">
-        <v>343</v>
+        <v>301</v>
       </c>
       <c r="H106" s="3"/>
     </row>
     <row r="107" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>344</v>
+        <v>302</v>
       </c>
       <c r="B107" t="s">
-        <v>345</v>
+        <v>303</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>346</v>
+        <v>304</v>
       </c>
       <c r="D107" t="s">
-        <v>347</v>
+        <v>305</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>348</v>
+        <v>306</v>
       </c>
       <c r="B108" t="s">
-        <v>349</v>
+        <v>307</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>350</v>
+        <v>308</v>
       </c>
       <c r="D108" t="s">
-        <v>351</v>
+        <v>309</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>374</v>
+        <v>322</v>
       </c>
       <c r="B109" t="s">
         <v>23</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>375</v>
+        <v>323</v>
       </c>
       <c r="D109" t="s">
-        <v>376</v>
+        <v>324</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>377</v>
+        <v>325</v>
       </c>
       <c r="B110" t="s">
-        <v>378</v>
+        <v>326</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>379</v>
+        <v>327</v>
       </c>
       <c r="D110" t="s">
-        <v>380</v>
+        <v>328</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>381</v>
+        <v>329</v>
       </c>
       <c r="B111" t="s">
-        <v>382</v>
+        <v>330</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>381</v>
+        <v>329</v>
       </c>
       <c r="D111" t="s">
-        <v>383</v>
+        <v>331</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>384</v>
+        <v>332</v>
       </c>
       <c r="B112" t="s">
-        <v>385</v>
+        <v>333</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>386</v>
+        <v>334</v>
       </c>
       <c r="D112" t="s">
-        <v>387</v>
+        <v>335</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>388</v>
+        <v>336</v>
       </c>
       <c r="B113" t="s">
-        <v>389</v>
+        <v>337</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>390</v>
+        <v>338</v>
       </c>
       <c r="D113" t="s">
-        <v>391</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>